<commit_message>
Renamed MenuDisplayModule to MenusInputOutputModule Added I/O handling for main menu option 0 -- Exit the program Reworked mainBeerGardenMenu module to accept user input ** Added Distributor Matcher Class to show which distributors are available to each brewery based on location within KY
</commit_message>
<xml_diff>
--- a/data/BreweryBackgroundDataset.xlsx
+++ b/data/BreweryBackgroundDataset.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redhe\IdeaProjects\Craft Brew Rate and Review\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redhe\IdeaProjects\CraftBrewRateReview\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{012162F3-3F5D-481C-87C5-36A58E0D65AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB49E93-8AF9-4712-BDA3-818D735675F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F96B66E8-DBB7-4B9A-A7F4-865DCAE86F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1389,7 +1390,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3272,4 +3273,29 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF313848-18C7-402B-901F-1F1FA3F7F0BF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A202" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H214" sqref="A1:H214"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="8"/>
+    <col min="2" max="2" width="52.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="8"/>
+    <col min="6" max="6" width="5.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="14.5703125" style="8"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>